<commit_message>
new source documents uploaded
</commit_message>
<xml_diff>
--- a/sources/Scheepstypenlijst.xlsx
+++ b/sources/Scheepstypenlijst.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="8385" yWindow="-15" windowWidth="15480" windowHeight="11640"/>
@@ -11,7 +11,7 @@
     <sheet name="Blad2" sheetId="2" r:id="rId2"/>
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -808,8 +808,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -874,7 +874,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -887,9 +887,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -927,7 +927,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -961,7 +961,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -996,10 +995,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1172,24 +1170,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" customWidth="1"/>
-    <col min="5" max="5" width="108.28515625" customWidth="1"/>
-    <col min="6" max="6" width="65.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="118.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1209,7 +1207,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -1217,7 +1215,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -1225,7 +1223,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -1233,7 +1231,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1250,7 +1248,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -1261,7 +1259,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1278,7 +1276,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>194</v>
       </c>
@@ -1292,7 +1290,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1309,7 +1307,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="B11" t="s">
         <v>15</v>
       </c>
@@ -1317,7 +1315,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="B12" t="s">
         <v>16</v>
       </c>
@@ -1331,7 +1329,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="B13" t="s">
         <v>17</v>
       </c>
@@ -1339,7 +1337,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>200</v>
       </c>
@@ -1356,7 +1354,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="B15" t="s">
         <v>19</v>
       </c>
@@ -1370,7 +1368,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="B16" t="s">
         <v>20</v>
       </c>
@@ -1378,7 +1376,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>125</v>
       </c>
@@ -1398,7 +1396,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="B18" t="s">
         <v>22</v>
       </c>
@@ -1406,7 +1404,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="B19" t="s">
         <v>23</v>
       </c>
@@ -1414,7 +1412,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>135</v>
       </c>
@@ -1434,7 +1432,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>127</v>
       </c>
@@ -1451,7 +1449,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="B22" t="s">
         <v>26</v>
       </c>
@@ -1465,7 +1463,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="B23" t="s">
         <v>27</v>
       </c>
@@ -1473,7 +1471,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="B24" t="s">
         <v>28</v>
       </c>
@@ -1481,7 +1479,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="B25" t="s">
         <v>29</v>
       </c>
@@ -1489,7 +1487,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>111</v>
       </c>
@@ -1509,7 +1507,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>111</v>
       </c>
@@ -1523,7 +1521,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1543,7 +1541,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1557,7 +1555,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1574,7 +1572,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1594,7 +1592,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="B32" t="s">
         <v>36</v>
       </c>
@@ -1602,12 +1600,12 @@
         <v>227</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="B33" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="B34" t="s">
         <v>38</v>
       </c>
@@ -1615,7 +1613,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="B35" t="s">
         <v>39</v>
       </c>
@@ -1623,7 +1621,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -1640,7 +1638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>126</v>
       </c>
@@ -1660,7 +1658,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="B38" t="s">
         <v>42</v>
       </c>
@@ -1668,7 +1666,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>116</v>
       </c>
@@ -1685,7 +1683,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="B40" t="s">
         <v>44</v>
       </c>
@@ -1693,7 +1691,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -1710,7 +1708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="B42" t="s">
         <v>46</v>
       </c>
@@ -1718,7 +1716,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6">
       <c r="B43" t="s">
         <v>47</v>
       </c>
@@ -1726,7 +1724,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>146</v>
       </c>
@@ -1743,7 +1741,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6">
       <c r="B45" t="s">
         <v>49</v>
       </c>
@@ -1757,7 +1755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6">
       <c r="B46" t="s">
         <v>50</v>
       </c>
@@ -1771,7 +1769,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6">
       <c r="B47" t="s">
         <v>51</v>
       </c>
@@ -1785,7 +1783,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6">
       <c r="B48" t="s">
         <v>52</v>
       </c>
@@ -1799,7 +1797,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="B49" t="s">
         <v>53</v>
       </c>
@@ -1807,7 +1805,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>54</v>
       </c>
@@ -1824,7 +1822,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>55</v>
       </c>
@@ -1841,7 +1839,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="B52" t="s">
         <v>56</v>
       </c>
@@ -1855,7 +1853,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>57</v>
       </c>
@@ -1872,7 +1870,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6">
       <c r="B54" t="s">
         <v>58</v>
       </c>
@@ -1889,7 +1887,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6">
       <c r="B55" t="s">
         <v>59</v>
       </c>
@@ -1903,7 +1901,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6">
       <c r="B56" t="s">
         <v>60</v>
       </c>
@@ -1911,7 +1909,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6">
       <c r="B57" t="s">
         <v>61</v>
       </c>
@@ -1919,7 +1917,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
         <v>62</v>
       </c>
@@ -1936,7 +1934,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
         <v>63</v>
       </c>
@@ -1953,7 +1951,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
         <v>161</v>
       </c>
@@ -1970,7 +1968,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
         <v>160</v>
       </c>
@@ -1987,7 +1985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
         <v>163</v>
       </c>
@@ -2001,7 +1999,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6">
       <c r="B63" t="s">
         <v>66</v>
       </c>
@@ -2012,7 +2010,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6">
       <c r="B64" t="s">
         <v>67</v>
       </c>
@@ -2020,7 +2018,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6">
       <c r="B65" t="s">
         <v>68</v>
       </c>
@@ -2028,7 +2026,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6">
       <c r="A66" t="s">
         <v>69</v>
       </c>
@@ -2048,7 +2046,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6">
       <c r="B67" t="s">
         <v>70</v>
       </c>
@@ -2056,7 +2054,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6">
       <c r="B68" t="s">
         <v>71</v>
       </c>
@@ -2064,7 +2062,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6">
       <c r="A69" t="s">
         <v>72</v>
       </c>
@@ -2081,7 +2079,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6">
       <c r="B70" t="s">
         <v>73</v>
       </c>
@@ -2095,7 +2093,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6">
       <c r="B71" t="s">
         <v>74</v>
       </c>
@@ -2109,7 +2107,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6">
       <c r="A72" t="s">
         <v>75</v>
       </c>
@@ -2126,7 +2124,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6">
       <c r="B73" t="s">
         <v>76</v>
       </c>
@@ -2134,7 +2132,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6">
       <c r="A74" t="s">
         <v>197</v>
       </c>
@@ -2151,7 +2149,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6">
       <c r="B75" t="s">
         <v>78</v>
       </c>
@@ -2159,7 +2157,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6">
       <c r="A76" t="s">
         <v>198</v>
       </c>
@@ -2176,7 +2174,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6">
       <c r="B77" t="s">
         <v>80</v>
       </c>
@@ -2184,7 +2182,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6">
       <c r="B78" t="s">
         <v>81</v>
       </c>
@@ -2192,7 +2190,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6">
       <c r="A79" t="s">
         <v>82</v>
       </c>
@@ -2209,7 +2207,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6">
       <c r="A80" t="s">
         <v>82</v>
       </c>
@@ -2226,7 +2224,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6">
       <c r="B81" t="s">
         <v>84</v>
       </c>
@@ -2234,7 +2232,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6">
       <c r="A82" t="s">
         <v>128</v>
       </c>
@@ -2251,7 +2249,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6">
       <c r="B83" t="s">
         <v>86</v>
       </c>
@@ -2259,7 +2257,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6">
       <c r="A84" t="s">
         <v>87</v>
       </c>
@@ -2276,7 +2274,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6">
       <c r="A85" t="s">
         <v>88</v>
       </c>
@@ -2293,7 +2291,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6">
       <c r="A86" t="s">
         <v>89</v>
       </c>
@@ -2310,7 +2308,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6">
       <c r="B87" t="s">
         <v>90</v>
       </c>
@@ -2318,7 +2316,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6">
       <c r="A88" t="s">
         <v>91</v>
       </c>
@@ -2335,7 +2333,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6">
       <c r="B89" t="s">
         <v>92</v>
       </c>
@@ -2343,7 +2341,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6">
       <c r="B90" t="s">
         <v>93</v>
       </c>
@@ -2351,7 +2349,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6">
       <c r="B91" t="s">
         <v>94</v>
       </c>
@@ -2359,7 +2357,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6">
       <c r="A92" t="s">
         <v>95</v>
       </c>
@@ -2376,7 +2374,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6">
       <c r="B93" t="s">
         <v>96</v>
       </c>
@@ -2384,7 +2382,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6">
       <c r="A94" t="s">
         <v>186</v>
       </c>
@@ -2401,7 +2399,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6">
       <c r="A95" t="s">
         <v>98</v>
       </c>
@@ -2418,7 +2416,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6">
       <c r="A96" t="s">
         <v>188</v>
       </c>
@@ -2435,7 +2433,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6">
       <c r="A97" t="s">
         <v>100</v>
       </c>
@@ -2452,7 +2450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6">
       <c r="B98" t="s">
         <v>101</v>
       </c>
@@ -2460,7 +2458,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6">
       <c r="A99" t="s">
         <v>100</v>
       </c>
@@ -2477,87 +2475,87 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6">
       <c r="C101" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6">
       <c r="C102" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6">
       <c r="C103" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6">
       <c r="C104" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6">
       <c r="C105" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6">
       <c r="C106" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6">
       <c r="C107" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6">
       <c r="C108" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6">
       <c r="C109" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6">
       <c r="C110" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6">
       <c r="C111" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6">
       <c r="C112" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:3">
       <c r="C113" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:3">
       <c r="C114" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:3">
       <c r="C115" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:3">
       <c r="C116" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="264" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="264" spans="6:6">
       <c r="F264" s="2"/>
     </row>
   </sheetData>
@@ -2570,24 +2568,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>